<commit_message>
changed col 4 and 5 name
</commit_message>
<xml_diff>
--- a/cost_recovery_record_from_2025.xlsx
+++ b/cost_recovery_record_from_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsrisai\Documents\TPSR core inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283004C1-E160-45E8-8ADD-D48A8FB3E4EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DC3BFC-019D-4485-BE71-F43A8C58117B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A65C8BF4-CB96-401D-8F12-F9A2BDA0DEB4}"/>
   </bookViews>
@@ -71,12 +71,6 @@
     <t>FFPE sectioning &amp; H&amp;E stain</t>
   </si>
   <si>
-    <t>Frozen sectioning &amp; H&amp;E slide</t>
-  </si>
-  <si>
-    <t>Repository FFPE sectioning &amp; H&amp;E stain</t>
-  </si>
-  <si>
     <t>Repository FFPE sectioning-unstained slide</t>
   </si>
   <si>
@@ -96,6 +90,12 @@
   </si>
   <si>
     <t>Requester_Name</t>
+  </si>
+  <si>
+    <t>Frozen sectioning &amp; H&amp;E stain</t>
+  </si>
+  <si>
+    <t>Frozen sectioning-unstained slide</t>
   </si>
 </sst>
 </file>
@@ -485,7 +485,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D03DD13-4E3A-4CD6-879D-A1B2A04A1C17}">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -495,7 +497,7 @@
     <col min="4" max="4" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.5703125" customWidth="1"/>
     <col min="8" max="8" width="37.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="41" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
@@ -503,16 +505,16 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>9</v>
@@ -521,13 +523,13 @@
         <v>10</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>6</v>
@@ -542,7 +544,7 @@
         <v>45948</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
@@ -566,7 +568,7 @@
         <v>45915</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -589,7 +591,7 @@
         <v>46071</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1">
         <v>250</v>
@@ -609,7 +611,7 @@
         <v>46076</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1">
         <v>2691</v>
@@ -632,7 +634,7 @@
         <v>46071</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D6" s="1">
         <v>254</v>
@@ -655,7 +657,7 @@
         <v>46072</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="N7" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
assigned unique color to requesters
</commit_message>
<xml_diff>
--- a/cost_recovery_record_from_2025.xlsx
+++ b/cost_recovery_record_from_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsrisai\Documents\TPSR core inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349244D1-3AA1-4C98-BC5D-7FD9CB1604F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46607B79-05C0-4E15-9D9B-39366D44FC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A65C8BF4-CB96-401D-8F12-F9A2BDA0DEB4}"/>
   </bookViews>
@@ -501,7 +501,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added cancer related project column
</commit_message>
<xml_diff>
--- a/cost_recovery_record_from_2025.xlsx
+++ b/cost_recovery_record_from_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsrisai\Documents\TPSR core inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46607B79-05C0-4E15-9D9B-39366D44FC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4298BB-86EB-4502-826F-6109C0EBDDCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A65C8BF4-CB96-401D-8F12-F9A2BDA0DEB4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>Dr. Awadh Binhazim</t>
   </si>
@@ -107,10 +107,19 @@
     <t>Dr. Sanford Barsky</t>
   </si>
   <si>
-    <t>breast cancer cell line</t>
-  </si>
-  <si>
     <t>tissue type</t>
+  </si>
+  <si>
+    <t>Breast cancer cell line</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Cancer_Related_Project</t>
   </si>
 </sst>
 </file>
@@ -498,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D03DD13-4E3A-4CD6-879D-A1B2A04A1C17}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,7 +527,7 @@
     <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -556,10 +565,13 @@
         <v>21</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -582,8 +594,11 @@
       <c r="M2" t="s">
         <v>6</v>
       </c>
+      <c r="N2" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -605,8 +620,11 @@
       <c r="M3" t="s">
         <v>6</v>
       </c>
+      <c r="N3" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -619,17 +637,17 @@
       <c r="D4" s="1">
         <v>250</v>
       </c>
-      <c r="G4">
-        <v>276</v>
-      </c>
       <c r="J4">
         <v>10</v>
       </c>
       <c r="M4" t="s">
         <v>7</v>
       </c>
+      <c r="N4" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -642,11 +660,20 @@
       <c r="D5" s="1">
         <v>2691</v>
       </c>
+      <c r="G5">
+        <v>276</v>
+      </c>
+      <c r="I5">
+        <v>276</v>
+      </c>
       <c r="M5" t="s">
         <v>6</v>
       </c>
+      <c r="N5" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -668,8 +695,11 @@
       <c r="M6" t="s">
         <v>6</v>
       </c>
+      <c r="N6" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -682,8 +712,11 @@
       <c r="M7" t="s">
         <v>6</v>
       </c>
+      <c r="N7" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -694,12 +727,10 @@
         <v>13</v>
       </c>
       <c r="M8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M9" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="N8" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>